<commit_message>
RE: Data Length Exceeded in schema validation issue for cs_pkpl_iec
Changed PACK_CLAS to VARCHAR2(5) for all of CCB_CS_PKPL_XXX same as CCB_CS_PKPL_PCN
</commit_message>
<xml_diff>
--- a/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.0.xlsx
+++ b/DTAC-SOURCE-TO-TARGET-MAPPING_SET2_V1.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_STM_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telenor-AEP\Requirement-Docs\DTAC_Sprint1_SS_Feeds\IS_DTAC_Feeds\Review_Feb2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Document - Sign-off" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Column Definition" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CCB!$A$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CCB!$A$1:$HF$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="276">
   <si>
     <t>Mode of Integration</t>
   </si>
@@ -882,6 +882,12 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR2(5) </t>
+  </si>
+  <si>
+    <t>VARCHAR2(5)</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:F28"/>
     </sheetView>
   </sheetViews>
@@ -2581,9 +2587,9 @@
   </sheetPr>
   <dimension ref="A1:HF208"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -9574,8 +9580,8 @@
       <c r="I31" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="J31" s="75" t="s">
-        <v>171</v>
+      <c r="J31" t="s">
+        <v>274</v>
       </c>
       <c r="K31" s="75" t="s">
         <v>164</v>
@@ -17240,7 +17246,7 @@
         <v>212</v>
       </c>
       <c r="J70" s="75" t="s">
-        <v>153</v>
+        <v>274</v>
       </c>
       <c r="K70" s="75" t="s">
         <v>164</v>
@@ -25289,7 +25295,7 @@
         <v>212</v>
       </c>
       <c r="J109" s="75" t="s">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="K109" s="75" t="s">
         <v>164</v>
@@ -43982,7 +43988,7 @@
       <c r="V208" s="124"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1"/>
+  <autoFilter ref="A1:HF1"/>
   <hyperlinks>
     <hyperlink ref="N38" location="'File_Date Reference'!A1" display="Refer to logic in document in Sheet &quot;File_Date_Reference&quot; Case No. &quot;01&quot;"/>
     <hyperlink ref="N77" location="'File_Date Reference'!A1" display="Refer to logic in document in Sheet &quot;File_Date_Reference&quot; Case No. &quot;01&quot;"/>
@@ -44854,12 +44860,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45080,15 +45083,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C16B0E6-E226-461B-8D00-37FDE1E9DF80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70785B63-45C8-4C04-9C8C-D6290BDFADA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fb15ab9c-5ce3-4966-97a0-841ffe55082a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45113,18 +45128,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70785B63-45C8-4C04-9C8C-D6290BDFADA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C16B0E6-E226-461B-8D00-37FDE1E9DF80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fb15ab9c-5ce3-4966-97a0-841ffe55082a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5c6a5f84-dc80-404b-9608-a58c80d813cf"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>